<commit_message>
updated model and iterations file/excel
</commit_message>
<xml_diff>
--- a/Model_Iterations.xlsx
+++ b/Model_Iterations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lijahoffman/Desktop/Bootcamp/git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lijahoffman/Desktop/Bootcamp/git/Off_to_the_Races/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF6B1D6-B117-2440-A1DE-1178EA774FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99A2B84-89B2-5649-BAC8-87AC42EDA7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="1240" windowWidth="27640" windowHeight="16000" xr2:uid="{D5E7FC4C-813C-CB49-8CC3-37D3351CB051}"/>
+    <workbookView xWindow="2840" yWindow="4400" windowWidth="27640" windowHeight="16000" xr2:uid="{D5E7FC4C-813C-CB49-8CC3-37D3351CB051}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Iteration</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Encoder used, additional features dropped (cleaning)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standaridizes data using standard scalar. Tests lasso and ridge regressions (multivariate linear regression still the best in terms of predicitve power). </t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8476AF-2B02-E445-B973-C9249E19C698}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,6 +591,26 @@
         <v>15</v>
       </c>
     </row>
+    <row r="7" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.59389000000000003</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cleaned up model file
</commit_message>
<xml_diff>
--- a/Model_Iterations.xlsx
+++ b/Model_Iterations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lijahoffman/Desktop/Bootcamp/git/Off_to_the_Races/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593E133B-0B87-A241-8C13-149C1C2AE453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F05D61F-5789-A64C-80E8-42D16FB457F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="3780" windowWidth="27640" windowHeight="16000" xr2:uid="{D5E7FC4C-813C-CB49-8CC3-37D3351CB051}"/>
+    <workbookView xWindow="1160" yWindow="1000" windowWidth="27640" windowHeight="16000" xr2:uid="{D5E7FC4C-813C-CB49-8CC3-37D3351CB051}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Iteration</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t xml:space="preserve">Standaridizes data using standard scalar. Tests lasso and ridge regressions (multivariate linear regression still the best in terms of predicitve power). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lasso and Ridge Regression performed for comparison. Ultimately decided that unscaled Linear Regression yielded the best results. </t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8476AF-2B02-E445-B973-C9249E19C698}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,6 +614,23 @@
         <v>18</v>
       </c>
     </row>
+    <row r="8" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>